<commit_message>
PUNTO DE PARTIDA: Solucionado el problema, sirve emisiones y blending
</commit_message>
<xml_diff>
--- a/Exported_files/Validacion_bau.xlsx
+++ b/Exported_files/Validacion_bau.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\Exported_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED0C23D-1CA4-46C5-94C0-FAA839D31DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3CA4B0-3A3B-4C14-9345-88BB2CAD401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$2:$N$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja2!$E$8:$R$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="29">
   <si>
     <t>Sum of Pv</t>
   </si>
@@ -116,6 +118,15 @@
   <si>
     <t>Period</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Table Name:</t>
+  </si>
+  <si>
+    <t>Unsaved_16342</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +156,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -342,7 +360,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -394,6 +412,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -3830,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA293C9-1FBB-4857-9FD3-79FCBBC8463C}">
   <dimension ref="A4:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9:X9"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D32:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4271,9 +4291,8 @@
         <f t="shared" si="2"/>
         <v>0.1627808307569063</v>
       </c>
-      <c r="X9" s="18">
-        <f t="shared" si="2"/>
-        <v>0.16256888734500968</v>
+      <c r="X9" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -4923,4 +4942,1301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5DAF1D-784F-4D3F-8E7D-EBA4A6AB59AE}">
+  <dimension ref="E7:AD28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18:AD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <v>28.366603784567701</v>
+      </c>
+      <c r="J9">
+        <v>27.490762332982001</v>
+      </c>
+      <c r="K9">
+        <v>27.7674957405642</v>
+      </c>
+      <c r="L9">
+        <v>28.166343684617399</v>
+      </c>
+      <c r="M9">
+        <v>28.871619909353701</v>
+      </c>
+      <c r="N9">
+        <v>29.733400650465899</v>
+      </c>
+      <c r="O9">
+        <v>30.685629483895799</v>
+      </c>
+      <c r="P9">
+        <v>31.4262868642226</v>
+      </c>
+      <c r="Q9">
+        <v>31.856649000215199</v>
+      </c>
+      <c r="R9">
+        <v>32.321972180891102</v>
+      </c>
+    </row>
+    <row r="10" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>28.366603784567701</v>
+      </c>
+      <c r="J10">
+        <v>27.490762332982001</v>
+      </c>
+      <c r="K10">
+        <v>27.7674957405642</v>
+      </c>
+      <c r="L10">
+        <v>28.166343684617399</v>
+      </c>
+      <c r="M10">
+        <v>28.871619909353701</v>
+      </c>
+      <c r="N10">
+        <v>29.733400650465899</v>
+      </c>
+      <c r="O10">
+        <v>30.685629483895799</v>
+      </c>
+      <c r="P10">
+        <v>31.4262868642226</v>
+      </c>
+      <c r="Q10">
+        <v>31.856649000215199</v>
+      </c>
+      <c r="R10">
+        <v>32.321972180891102</v>
+      </c>
+      <c r="U10">
+        <v>2019</v>
+      </c>
+      <c r="V10">
+        <v>2020</v>
+      </c>
+      <c r="W10">
+        <v>2023</v>
+      </c>
+      <c r="X10">
+        <v>2025</v>
+      </c>
+      <c r="Y10">
+        <v>2027</v>
+      </c>
+      <c r="Z10">
+        <v>2030</v>
+      </c>
+      <c r="AA10">
+        <v>2033</v>
+      </c>
+      <c r="AB10">
+        <v>2035</v>
+      </c>
+      <c r="AC10">
+        <v>2037</v>
+      </c>
+      <c r="AD10">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="11" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11">
+        <v>2.0905752518302898</v>
+      </c>
+      <c r="J11">
+        <v>1.8638264498142201</v>
+      </c>
+      <c r="K11">
+        <v>2.1381708371438402</v>
+      </c>
+      <c r="L11">
+        <v>2.32120154265407</v>
+      </c>
+      <c r="M11">
+        <v>2.5048142159459301</v>
+      </c>
+      <c r="N11">
+        <v>2.7813864099923</v>
+      </c>
+      <c r="O11">
+        <v>3.0836805722629599</v>
+      </c>
+      <c r="P11">
+        <v>3.28568473695444</v>
+      </c>
+      <c r="Q11">
+        <v>3.5087678306828498</v>
+      </c>
+      <c r="R11">
+        <v>3.8434999021949801</v>
+      </c>
+      <c r="T11" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="19">
+        <f>+I11/(I11+I21)</f>
+        <v>9.3659149944684203E-2</v>
+      </c>
+      <c r="V11" s="19">
+        <f t="shared" ref="V11:AD11" si="0">+J11/(J11+J21)</f>
+        <v>9.3659149944684605E-2</v>
+      </c>
+      <c r="W11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944684258E-2</v>
+      </c>
+      <c r="X11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944683884E-2</v>
+      </c>
+      <c r="Y11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.365914994468412E-2</v>
+      </c>
+      <c r="Z11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944684467E-2</v>
+      </c>
+      <c r="AA11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.365914994468405E-2</v>
+      </c>
+      <c r="AB11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944683814E-2</v>
+      </c>
+      <c r="AC11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944683814E-2</v>
+      </c>
+      <c r="AD11" s="19">
+        <f t="shared" si="0"/>
+        <v>9.3659149944683759E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <v>2.0905752518302898</v>
+      </c>
+      <c r="J12">
+        <v>1.8638264498142201</v>
+      </c>
+      <c r="K12">
+        <v>2.7906948896535702</v>
+      </c>
+      <c r="L12">
+        <v>3.5014886319771699</v>
+      </c>
+      <c r="M12">
+        <v>3.77837625503166</v>
+      </c>
+      <c r="N12">
+        <v>4.1954234127820804</v>
+      </c>
+      <c r="O12">
+        <v>4.6512861260941198</v>
+      </c>
+      <c r="P12">
+        <v>4.9558982406941503</v>
+      </c>
+      <c r="Q12">
+        <v>5.2923263461571004</v>
+      </c>
+      <c r="R12">
+        <v>5.79711747856736</v>
+      </c>
+      <c r="T12" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="19">
+        <f>+I12/(I12+I22)</f>
+        <v>9.3659149944684203E-2</v>
+      </c>
+      <c r="V12" s="19">
+        <f t="shared" ref="V12:AD12" si="1">+J12/(J12+J22)</f>
+        <v>9.3659149944684605E-2</v>
+      </c>
+      <c r="W12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.12222008510205448</v>
+      </c>
+      <c r="X12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.1412410114674324</v>
+      </c>
+      <c r="Y12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.14123816660250149</v>
+      </c>
+      <c r="Z12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.14123391748640046</v>
+      </c>
+      <c r="AA12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.1412309020220027</v>
+      </c>
+      <c r="AB12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.14122889649492057</v>
+      </c>
+      <c r="AC12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.14122763811848157</v>
+      </c>
+      <c r="AD12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.14122575115394595</v>
+      </c>
+    </row>
+    <row r="13" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>0.24035823080041199</v>
+      </c>
+      <c r="J13">
+        <v>0.20514844055110801</v>
+      </c>
+      <c r="K13">
+        <v>0.22795380282151001</v>
+      </c>
+      <c r="L13">
+        <v>0.24358673712875101</v>
+      </c>
+      <c r="M13">
+        <v>0.254316444069555</v>
+      </c>
+      <c r="N13">
+        <v>0.270373544733089</v>
+      </c>
+      <c r="O13">
+        <v>0.282252030680748</v>
+      </c>
+      <c r="P13">
+        <v>0.289939231876707</v>
+      </c>
+      <c r="Q13">
+        <v>0.31039829515325901</v>
+      </c>
+      <c r="R13">
+        <v>0.32198206861256901</v>
+      </c>
+      <c r="T13" t="s">
+        <v>21</v>
+      </c>
+      <c r="U13" s="19">
+        <f>+I13/(I13+I23)</f>
+        <v>9.5093460516067332E-2</v>
+      </c>
+      <c r="V13" s="19">
+        <f t="shared" ref="V13:AD13" si="2">+J13/(J13+J23)</f>
+        <v>9.5258376927519192E-2</v>
+      </c>
+      <c r="W13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5233819400142888E-2</v>
+      </c>
+      <c r="X13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5218019360781003E-2</v>
+      </c>
+      <c r="Y13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5194192868011965E-2</v>
+      </c>
+      <c r="Z13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5158393951040032E-2</v>
+      </c>
+      <c r="AA13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5151185228618179E-2</v>
+      </c>
+      <c r="AB13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.5146271084799075E-2</v>
+      </c>
+      <c r="AC13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.8781534925760278E-2</v>
+      </c>
+      <c r="AD13" s="19">
+        <f t="shared" si="2"/>
+        <v>9.8729787134684194E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>0.24035823080041199</v>
+      </c>
+      <c r="J14">
+        <v>0.20514844055110801</v>
+      </c>
+      <c r="K14">
+        <v>0.30000847152499599</v>
+      </c>
+      <c r="L14">
+        <v>0.37014232269141001</v>
+      </c>
+      <c r="M14">
+        <v>0.38646685123955499</v>
+      </c>
+      <c r="N14">
+        <v>0.41089998382354398</v>
+      </c>
+      <c r="O14">
+        <v>0.42891554058451897</v>
+      </c>
+      <c r="P14">
+        <v>0.44057141041458597</v>
+      </c>
+      <c r="Q14">
+        <v>0.465064630933196</v>
+      </c>
+      <c r="R14">
+        <v>0.48245555033347598</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="19">
+        <f>+I14/(I14+I24)</f>
+        <v>9.5093460516067332E-2</v>
+      </c>
+      <c r="V14" s="19">
+        <f t="shared" ref="V14:AD14" si="3">+J14/(J14+J24)</f>
+        <v>9.5258376927519192E-2</v>
+      </c>
+      <c r="W14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.1251670702815236</v>
+      </c>
+      <c r="X14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14436725564549791</v>
+      </c>
+      <c r="Y14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14433954729743284</v>
+      </c>
+      <c r="Z14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14429791532592182</v>
+      </c>
+      <c r="AA14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14427699573634528</v>
+      </c>
+      <c r="AB14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14426273457951044</v>
+      </c>
+      <c r="AC14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14768338089581823</v>
+      </c>
+      <c r="AD14" s="20">
+        <f t="shared" si="3"/>
+        <v>0.14761937697198937</v>
+      </c>
+    </row>
+    <row r="15" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>22.938985434840198</v>
+      </c>
+      <c r="J15">
+        <v>23.722780815627399</v>
+      </c>
+      <c r="K15">
+        <v>25.608296081752901</v>
+      </c>
+      <c r="L15">
+        <v>26.8690760104971</v>
+      </c>
+      <c r="M15">
+        <v>27.6869064108438</v>
+      </c>
+      <c r="N15">
+        <v>28.821083964343298</v>
+      </c>
+      <c r="O15">
+        <v>29.267723732473701</v>
+      </c>
+      <c r="P15">
+        <v>29.549667857678202</v>
+      </c>
+      <c r="Q15">
+        <v>29.4823389390545</v>
+      </c>
+      <c r="R15">
+        <v>29.333643028329899</v>
+      </c>
+      <c r="T15" t="s">
+        <v>21</v>
+      </c>
+      <c r="U15" s="19">
+        <f>+I15/(I15+I25)</f>
+        <v>9.3774378982327933E-2</v>
+      </c>
+      <c r="V15" s="19">
+        <f t="shared" ref="V15:AD15" si="4">+J15/(J15+J25)</f>
+        <v>9.3768415272765568E-2</v>
+      </c>
+      <c r="W15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3773465964128666E-2</v>
+      </c>
+      <c r="X15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3776823067369064E-2</v>
+      </c>
+      <c r="Y15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3832987720932307E-2</v>
+      </c>
+      <c r="Z15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3659149944684911E-2</v>
+      </c>
+      <c r="AA15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3659149944685716E-2</v>
+      </c>
+      <c r="AB15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3659149944685577E-2</v>
+      </c>
+      <c r="AC15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3659149944684494E-2</v>
+      </c>
+      <c r="AD15" s="19">
+        <f t="shared" si="4"/>
+        <v>9.3659149944682857E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>22.938985434840198</v>
+      </c>
+      <c r="J16">
+        <v>23.722780815627399</v>
+      </c>
+      <c r="K16">
+        <v>38.3989486395526</v>
+      </c>
+      <c r="L16">
+        <v>49.208937033772401</v>
+      </c>
+      <c r="M16">
+        <v>50.592374533080203</v>
+      </c>
+      <c r="N16">
+        <v>52.557714146922898</v>
+      </c>
+      <c r="O16">
+        <v>53.270978702205603</v>
+      </c>
+      <c r="P16">
+        <v>53.714200547616002</v>
+      </c>
+      <c r="Q16">
+        <v>53.596150990900902</v>
+      </c>
+      <c r="R16">
+        <v>53.3326814656793</v>
+      </c>
+      <c r="T16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="19">
+        <f>+I16/(I16+I26)</f>
+        <v>9.3774378982327933E-2</v>
+      </c>
+      <c r="V16" s="19">
+        <f t="shared" ref="V16:AD16" si="5">+J16/(J16+J26)</f>
+        <v>9.3768415272765568E-2</v>
+      </c>
+      <c r="W16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.13806873958818841</v>
+      </c>
+      <c r="X16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16663871863601928</v>
+      </c>
+      <c r="Y16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16641702669041705</v>
+      </c>
+      <c r="Z16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16585143002554859</v>
+      </c>
+      <c r="AA16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16558897429117714</v>
+      </c>
+      <c r="AB16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16540923097984905</v>
+      </c>
+      <c r="AC16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16542040587945628</v>
+      </c>
+      <c r="AD16" s="20">
+        <f t="shared" si="5"/>
+        <v>0.16543812879281902</v>
+      </c>
+    </row>
+    <row r="17" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17">
+        <v>25.2699189174709</v>
+      </c>
+      <c r="J17">
+        <v>25.791755705992699</v>
+      </c>
+      <c r="K17">
+        <v>27.9744207217182</v>
+      </c>
+      <c r="L17">
+        <v>29.433864290279899</v>
+      </c>
+      <c r="M17">
+        <v>30.446037070859301</v>
+      </c>
+      <c r="N17">
+        <v>31.8728439190687</v>
+      </c>
+      <c r="O17">
+        <v>32.633656335417399</v>
+      </c>
+      <c r="P17">
+        <v>33.125291826509397</v>
+      </c>
+      <c r="Q17">
+        <v>33.301505064890598</v>
+      </c>
+      <c r="R17">
+        <v>33.4991249991375</v>
+      </c>
+      <c r="T17" t="s">
+        <v>21</v>
+      </c>
+      <c r="U17" s="19">
+        <f>+I17/(I17+I27)</f>
+        <v>9.3777207046305044E-2</v>
+      </c>
+      <c r="V17" s="19">
+        <f t="shared" ref="V17:AD17" si="6">+J17/(J17+J27)</f>
+        <v>9.3772176049885039E-2</v>
+      </c>
+      <c r="W17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3776435302390673E-2</v>
+      </c>
+      <c r="X17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.37792780111842E-2</v>
+      </c>
+      <c r="Y17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3829867131587821E-2</v>
+      </c>
+      <c r="Z17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3671669152703307E-2</v>
+      </c>
+      <c r="AA17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3671854086912393E-2</v>
+      </c>
+      <c r="AB17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3671964734150293E-2</v>
+      </c>
+      <c r="AC17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3704440962917232E-2</v>
+      </c>
+      <c r="AD17" s="19">
+        <f t="shared" si="6"/>
+        <v>9.3705406917775638E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18">
+        <v>25.2699189174709</v>
+      </c>
+      <c r="J18">
+        <v>25.791755705992699</v>
+      </c>
+      <c r="K18">
+        <v>41.489652000731098</v>
+      </c>
+      <c r="L18">
+        <v>53.080567988440997</v>
+      </c>
+      <c r="M18">
+        <v>54.757217639351403</v>
+      </c>
+      <c r="N18">
+        <v>57.164037543528501</v>
+      </c>
+      <c r="O18">
+        <v>58.351180368884201</v>
+      </c>
+      <c r="P18">
+        <v>59.110670198724797</v>
+      </c>
+      <c r="Q18">
+        <v>59.353541967991198</v>
+      </c>
+      <c r="R18">
+        <v>59.612254494580199</v>
+      </c>
+      <c r="T18" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="19">
+        <f>+I18/(I18+I28)</f>
+        <v>9.3777207046305044E-2</v>
+      </c>
+      <c r="V18" s="19">
+        <f t="shared" ref="V18:AD18" si="7">+J18/(J18+J28)</f>
+        <v>9.3772176049885039E-2</v>
+      </c>
+      <c r="W18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.13677383899696285</v>
+      </c>
+      <c r="X18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.1645103557742689</v>
+      </c>
+      <c r="Y18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.16421964621465976</v>
+      </c>
+      <c r="Z18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.16358314542607813</v>
+      </c>
+      <c r="AA18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.16316857976953786</v>
+      </c>
+      <c r="AB18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.16289297912281925</v>
+      </c>
+      <c r="AC18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.1627808307569063</v>
+      </c>
+      <c r="AD18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.16256888734500968</v>
+      </c>
+    </row>
+    <row r="19" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>21.950277468988102</v>
+      </c>
+      <c r="J19">
+        <v>21.272545195249801</v>
+      </c>
+      <c r="K19">
+        <v>21.486683451894901</v>
+      </c>
+      <c r="L19">
+        <v>21.795314795512599</v>
+      </c>
+      <c r="M19">
+        <v>22.341062497381099</v>
+      </c>
+      <c r="N19">
+        <v>23.007914494486698</v>
+      </c>
+      <c r="O19">
+        <v>23.744755861415801</v>
+      </c>
+      <c r="P19">
+        <v>24.317881750263801</v>
+      </c>
+      <c r="Q19">
+        <v>24.6508989971971</v>
+      </c>
+      <c r="R19">
+        <v>25.010969346335699</v>
+      </c>
+    </row>
+    <row r="20" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>21.950277468988102</v>
+      </c>
+      <c r="J20">
+        <v>21.272545195249801</v>
+      </c>
+      <c r="K20">
+        <v>21.486683451894901</v>
+      </c>
+      <c r="L20">
+        <v>21.795314795512599</v>
+      </c>
+      <c r="M20">
+        <v>22.341062497381099</v>
+      </c>
+      <c r="N20">
+        <v>23.007914494486698</v>
+      </c>
+      <c r="O20">
+        <v>23.744755861415801</v>
+      </c>
+      <c r="P20">
+        <v>24.317881750263801</v>
+      </c>
+      <c r="Q20">
+        <v>24.6508989971971</v>
+      </c>
+      <c r="R20">
+        <v>25.010969346335699</v>
+      </c>
+    </row>
+    <row r="21" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21">
+        <v>20.230524748169699</v>
+      </c>
+      <c r="J21">
+        <v>18.0362735501858</v>
+      </c>
+      <c r="K21">
+        <v>20.691107865542001</v>
+      </c>
+      <c r="L21">
+        <v>22.462298457345899</v>
+      </c>
+      <c r="M21">
+        <v>24.239120759177101</v>
+      </c>
+      <c r="N21">
+        <v>26.915513590007698</v>
+      </c>
+      <c r="O21">
+        <v>29.840818252296199</v>
+      </c>
+      <c r="P21">
+        <v>31.795615263045601</v>
+      </c>
+      <c r="Q21">
+        <v>33.954393352769799</v>
+      </c>
+      <c r="R21">
+        <v>37.193600097805003</v>
+      </c>
+    </row>
+    <row r="22" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22">
+        <v>20.230524748169699</v>
+      </c>
+      <c r="J22">
+        <v>18.0362735501858</v>
+      </c>
+      <c r="K22">
+        <v>20.042662551746702</v>
+      </c>
+      <c r="L22">
+        <v>21.289389000505299</v>
+      </c>
+      <c r="M22">
+        <v>22.9734313188054</v>
+      </c>
+      <c r="N22">
+        <v>25.510071467270802</v>
+      </c>
+      <c r="O22">
+        <v>28.282626066645999</v>
+      </c>
+      <c r="P22">
+        <v>30.135349823206099</v>
+      </c>
+      <c r="Q22">
+        <v>32.181403418530699</v>
+      </c>
+      <c r="R22">
+        <v>35.251469136830401</v>
+      </c>
+    </row>
+    <row r="23" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23">
+        <v>2.2872417691995901</v>
+      </c>
+      <c r="J23">
+        <v>1.94845155944892</v>
+      </c>
+      <c r="K23">
+        <v>2.1656685915898599</v>
+      </c>
+      <c r="L23">
+        <v>2.3146132628712599</v>
+      </c>
+      <c r="M23">
+        <v>2.4172377380449799</v>
+      </c>
+      <c r="N23">
+        <v>2.5709264552668998</v>
+      </c>
+      <c r="O23">
+        <v>2.6841012522824199</v>
+      </c>
+      <c r="P23">
+        <v>2.7573607681232799</v>
+      </c>
+      <c r="Q23">
+        <v>2.8318721239745699</v>
+      </c>
+      <c r="R23">
+        <v>2.9392633767293801</v>
+      </c>
+    </row>
+    <row r="24" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24">
+        <v>2.2872417691995901</v>
+      </c>
+      <c r="J24">
+        <v>1.94845155944892</v>
+      </c>
+      <c r="K24">
+        <v>2.0968557424429601</v>
+      </c>
+      <c r="L24">
+        <v>2.1937515536340899</v>
+      </c>
+      <c r="M24">
+        <v>2.29101730660655</v>
+      </c>
+      <c r="N24">
+        <v>2.4366808900612602</v>
+      </c>
+      <c r="O24">
+        <v>2.54394606077796</v>
+      </c>
+      <c r="P24">
+        <v>2.61338019877084</v>
+      </c>
+      <c r="Q24">
+        <v>2.6840008096885302</v>
+      </c>
+      <c r="R24">
+        <v>2.7857844343470002</v>
+      </c>
+    </row>
+    <row r="25" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25">
+        <v>221.67991456516</v>
+      </c>
+      <c r="J25">
+        <v>229.270519184373</v>
+      </c>
+      <c r="K25">
+        <v>247.47850750881599</v>
+      </c>
+      <c r="L25">
+        <v>259.65242398950198</v>
+      </c>
+      <c r="M25">
+        <v>267.37890235554801</v>
+      </c>
+      <c r="N25">
+        <v>278.90201603565703</v>
+      </c>
+      <c r="O25">
+        <v>283.22415506163202</v>
+      </c>
+      <c r="P25">
+        <v>285.95253214232201</v>
+      </c>
+      <c r="Q25">
+        <v>285.30098929387202</v>
+      </c>
+      <c r="R25">
+        <v>283.86205697166997</v>
+      </c>
+    </row>
+    <row r="26" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26">
+        <v>221.67991456516</v>
+      </c>
+      <c r="J26">
+        <v>229.270519184373</v>
+      </c>
+      <c r="K26">
+        <v>239.71576982665101</v>
+      </c>
+      <c r="L26">
+        <v>246.09420401628</v>
+      </c>
+      <c r="M26">
+        <v>253.41723036868501</v>
+      </c>
+      <c r="N26">
+        <v>264.338643869566</v>
+      </c>
+      <c r="O26">
+        <v>268.43509460514002</v>
+      </c>
+      <c r="P26">
+        <v>271.02100455202998</v>
+      </c>
+      <c r="Q26">
+        <v>270.40348318940102</v>
+      </c>
+      <c r="R26">
+        <v>269.03968731557501</v>
+      </c>
+    </row>
+    <row r="27" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27">
+        <v>244.19768108252899</v>
+      </c>
+      <c r="J27">
+        <v>249.25524429400701</v>
+      </c>
+      <c r="K27">
+        <v>270.33528396594801</v>
+      </c>
+      <c r="L27">
+        <v>284.42933570972002</v>
+      </c>
+      <c r="M27">
+        <v>294.03526085277002</v>
+      </c>
+      <c r="N27">
+        <v>308.38845608093101</v>
+      </c>
+      <c r="O27">
+        <v>315.74907456621099</v>
+      </c>
+      <c r="P27">
+        <v>320.50550817349102</v>
+      </c>
+      <c r="Q27">
+        <v>322.08725477061603</v>
+      </c>
+      <c r="R27">
+        <v>323.99492044620399</v>
+      </c>
+    </row>
+    <row r="28" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28">
+        <v>244.19768108252899</v>
+      </c>
+      <c r="J28">
+        <v>249.25524429400701</v>
+      </c>
+      <c r="K28">
+        <v>261.85528812083999</v>
+      </c>
+      <c r="L28">
+        <v>269.57734457041897</v>
+      </c>
+      <c r="M28">
+        <v>278.68167899409701</v>
+      </c>
+      <c r="N28">
+        <v>292.28539622689902</v>
+      </c>
+      <c r="O28">
+        <v>299.26166673256398</v>
+      </c>
+      <c r="P28">
+        <v>303.76973457400697</v>
+      </c>
+      <c r="Q28">
+        <v>305.26888741762002</v>
+      </c>
+      <c r="R28">
+        <v>307.07694088675299</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="E8:R8" xr:uid="{2B5DAF1D-784F-4D3F-8E7D-EBA4A6AB59AE}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>